<commit_message>
Updated Excel file and save_reqs logic
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" tabRatio="907" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9000" tabRatio="907" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Design Operating Data" sheetId="23" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Key" sheetId="20" r:id="rId3"/>
     <sheet name="Boiler" sheetId="2" r:id="rId4"/>
     <sheet name="Heat Recovery Steam Gen" sheetId="26" r:id="rId5"/>
-    <sheet name="Steam Turbine" sheetId="3" r:id="rId6"/>
+    <sheet name="Steam Turbine " sheetId="3" r:id="rId6"/>
     <sheet name="Gas Turbine" sheetId="9" r:id="rId7"/>
     <sheet name="Generator" sheetId="4" r:id="rId8"/>
     <sheet name="Transformer" sheetId="12" r:id="rId9"/>
@@ -15174,7 +15174,7 @@
   <sheetPr/>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -16975,8 +16975,8 @@
   <sheetPr/>
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="4"/>

</xml_diff>